<commit_message>
integrated freezeaccount and excelmanager with main function
</commit_message>
<xml_diff>
--- a/src/models/frozenAccounts.xlsx
+++ b/src/models/frozenAccounts.xlsx
@@ -397,9 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -424,9 +424,20 @@
         <v>Pn53nwweUKzSZ7tZrsZ1wh3HCG3F9HGWthPwQUJpyGcydKaGxnpdzjqmUz34FGqh7acXWTvhK976rMNQmwucscP</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>3HkSLidfgeLyM1izEZMvB4eKHi94U4HWbBdfvY48Vpq3</v>
+      </c>
+      <c r="B3">
+        <v>0.2</v>
+      </c>
+      <c r="C3" t="str">
+        <v>2fAbEYKeY2yfGAAhNCB2bpg1ACR3PvVACGha3Z6FM8HuosYzNUYVhzN7oPT2aqwWQsYMuTTzSwWaiK1YYgAcH3AZ</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
tidyying up part 0
</commit_message>
<xml_diff>
--- a/src/models/frozenAccounts.xlsx
+++ b/src/models/frozenAccounts.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -435,9 +435,42 @@
         <v>2fAbEYKeY2yfGAAhNCB2bpg1ACR3PvVACGha3Z6FM8HuosYzNUYVhzN7oPT2aqwWQsYMuTTzSwWaiK1YYgAcH3AZ</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>3HkSLidfgeLyM1izEZMvB4eKHi94U4HWbBdfvY48Vpq3</v>
+      </c>
+      <c r="B4">
+        <v>0.2</v>
+      </c>
+      <c r="C4" t="str">
+        <v>5Lv2jkvax2bGZmPL7tsuDcdBJ72dtMSCaxXp1HVQkRrfDsyFqq9A98SmV9DsKm5m1f4kfWU6mKZTZPdHHnKzpG39</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>3HkSLidfgeLyM1izEZMvB4eKHi94U4HWbBdfvY48Vpq3</v>
+      </c>
+      <c r="B5">
+        <v>0.2</v>
+      </c>
+      <c r="C5" t="str">
+        <v>5mepBeyQa3hY5XvM2sWmdBkVCCEbeASmMbu95toqHM61Y22cFUxpksP1v8UTphorcG3vPtxgsX4JkB5rnLPox3rv</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>3HkSLidfgeLyM1izEZMvB4eKHi94U4HWbBdfvY48Vpq3</v>
+      </c>
+      <c r="B6">
+        <v>0.2</v>
+      </c>
+      <c r="C6" t="str">
+        <v>2Ng1fSefsqzd6ZwCwgmQU3yKQG7eVNWM68zDfomQV8Z2RWcP8kwp33gNXHfS9PrAbib136TAi7DBBwjXL3Bq3SXo</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactoring and debugging utils dir/
</commit_message>
<xml_diff>
--- a/src/models/frozenAccounts.xlsx
+++ b/src/models/frozenAccounts.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -468,9 +468,75 @@
         <v>2Ng1fSefsqzd6ZwCwgmQU3yKQG7eVNWM68zDfomQV8Z2RWcP8kwp33gNXHfS9PrAbib136TAi7DBBwjXL3Bq3SXo</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>ACzFALBrQjSkcqxWdGRx6x4eGZbf2RbwMtC7nS5ckBVP</v>
+      </c>
+      <c r="B7">
+        <v>90</v>
+      </c>
+      <c r="C7" t="str">
+        <v>asefuaihwefcbebn</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>ACzFALBrQjSkcqxWdGRx6x4eGZbf2RbwMtC7nS5ckBVP</v>
+      </c>
+      <c r="B8">
+        <v>90</v>
+      </c>
+      <c r="C8" t="str">
+        <v>asefuaihwefcbebn</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>ACzFALBrQjSkcqxWdGRx6x4eGZbf2RbwMtC7nS5ckBVP</v>
+      </c>
+      <c r="B9">
+        <v>90</v>
+      </c>
+      <c r="C9" t="str">
+        <v>asefuaihwefcbebn</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>ACzFALBrQjSkcqxWdGRx6x4eGZbf2RbwMtC7nS5ckBVP</v>
+      </c>
+      <c r="B10">
+        <v>90</v>
+      </c>
+      <c r="C10" t="str">
+        <v>asefuaihwefcbebn</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>ACzFALBrQjSkcqxWdGRx6x4eGZbf2RbwMtC7nS5ckBVP</v>
+      </c>
+      <c r="B11">
+        <v>90</v>
+      </c>
+      <c r="C11" t="str">
+        <v>56ZcbkWFcsBagDXNB8Yyk6nyCdTa6S8i71wVz3zdwVwvtgmAAJh1cVxyLx6P3FkwSRqawQHmQNgM2iitv3RoEM4</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>ACzFALBrQjSkcqxWdGRx6x4eGZbf2RbwMtC7nS5ckBVP</v>
+      </c>
+      <c r="B12">
+        <v>90</v>
+      </c>
+      <c r="C12" t="str">
+        <v>hHPtn2TXQMt1YcbMKTYLMf8hmR6NFekF3jyjRrMqNWr48ULoCG9cFeyTA98C2rBWcEf4kMuTW42tVoNw5eN7FHJ</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>